<commit_message>
updated on 25-12-22 at 12.45 pm
</commit_message>
<xml_diff>
--- a/com.tutorialsNinja/TestData/MyTestDataTDD.xlsx
+++ b/com.tutorialsNinja/TestData/MyTestDataTDD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14535" windowHeight="10575"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25260" windowHeight="8760"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
@@ -374,7 +374,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -397,7 +397,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1">
@@ -409,7 +409,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>123456</v>
@@ -420,8 +420,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>